<commit_message>
update result 20200914 at am 10:00
</commit_message>
<xml_diff>
--- a/20200912.xlsx
+++ b/20200912.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3553E502-BF1C-43FE-A834-53EBF5D6DE8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B90BCA-2DB0-400B-9C05-6F587377C86C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1365" windowWidth="27000" windowHeight="14235" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>소요시간</t>
   </si>
@@ -207,6 +207,14 @@
   </si>
   <si>
     <t>30분 늦잠 잤다</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>6시 이후 자유시간 가짐</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>일요일 계획 작성을 안함</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -937,99 +945,102 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1564,7 +1575,7 @@
   <dimension ref="B2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1578,19 +1589,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="31" t="s">
         <v>52</v>
       </c>
       <c r="H2" t="s">
@@ -1610,17 +1621,17 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="24" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="15"/>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="18" t="s">
         <v>55</v>
       </c>
       <c r="H3" t="s">
@@ -1634,11 +1645,11 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="12"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="19"/>
       <c r="H4" t="s">
         <v>20</v>
       </c>
@@ -1647,11 +1658,11 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="11"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="20"/>
       <c r="H5" t="s">
         <v>23</v>
       </c>
@@ -1660,11 +1671,11 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="30"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="14"/>
       <c r="H6" t="s">
         <v>24</v>
       </c>
@@ -1673,11 +1684,11 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="30"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="14"/>
       <c r="H7" t="s">
         <v>9</v>
       </c>
@@ -1690,11 +1701,11 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="30"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="14"/>
       <c r="H8" t="s">
         <v>11</v>
       </c>
@@ -1703,15 +1714,15 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="14" t="s">
+      <c r="D9" s="24"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="18" t="s">
         <v>56</v>
       </c>
       <c r="H9" t="s">
@@ -1720,167 +1731,171 @@
       <c r="I9">
         <v>309</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="2:12" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="18" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="2:6" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="19"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="2"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="29" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
@@ -1891,7 +1906,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="D19:D23"/>
+    <mergeCell ref="F18:F21"/>
     <mergeCell ref="E3:E5"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="F9:F11"/>
@@ -1899,7 +1916,6 @@
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D10"/>
     <mergeCell ref="D11:D18"/>
-    <mergeCell ref="D19:D23"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69999998807907104" right="0.69999998807907104" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>